<commit_message>
Updated Gerbers for Sprite
</commit_message>
<xml_diff>
--- a/Sprite/EagleCAD/Sprite/Sprite_Files/SpriteBOM.xlsx
+++ b/Sprite/EagleCAD/Sprite/Sprite_Files/SpriteBOM.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="0" windowWidth="24760" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24760" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="SpriteBOM" localSheetId="0">Sheet1!$A$1:$G$29</definedName>
+    <definedName name="SpriteBOM" localSheetId="0">Sheet1!$A$1:$G$31</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="126">
   <si>
     <t>Part</t>
   </si>
@@ -117,9 +117,6 @@
     <t>220nF</t>
   </si>
   <si>
-    <t>C13</t>
-  </si>
-  <si>
     <t>4.7uF</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>Inductors</t>
   </si>
   <si>
-    <t>LED1</t>
-  </si>
-  <si>
     <t>LED0603</t>
   </si>
   <si>
@@ -405,12 +399,6 @@
     <t>Test Pin</t>
   </si>
   <si>
-    <t>On Hand</t>
-  </si>
-  <si>
-    <t>On Order</t>
-  </si>
-  <si>
     <t>ED1088CT-ND</t>
   </si>
   <si>
@@ -418,6 +406,18 @@
   </si>
   <si>
     <t>0603-IND</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R10</t>
   </si>
 </sst>
 </file>
@@ -503,8 +503,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -523,9 +525,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -859,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -876,7 +880,7 @@
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -893,19 +897,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -922,18 +920,15 @@
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -948,18 +943,15 @@
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J3">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -974,18 +966,15 @@
         <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J4">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -1000,18 +989,15 @@
         <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -1026,18 +1012,15 @@
         <v>9</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -1052,18 +1035,15 @@
         <v>9</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
@@ -1078,18 +1058,15 @@
         <v>9</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J8">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -1104,18 +1081,15 @@
         <v>9</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J9">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -1130,18 +1104,15 @@
         <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J10">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
@@ -1156,18 +1127,15 @@
         <v>9</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J11">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
@@ -1182,21 +1150,18 @@
         <v>9</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J12">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
         <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -1208,526 +1173,509 @@
         <v>9</v>
       </c>
       <c r="F13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="J13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
         <v>125</v>
       </c>
-      <c r="E14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="J14">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
         <v>37</v>
       </c>
-      <c r="E15" t="s">
+      <c r="B32" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="J15">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="J16">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="J17">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="J18">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="J19">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="J20">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="J21">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="J22">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="J23">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" t="s">
-        <v>115</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" t="s">
-        <v>115</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="I26">
-        <v>40</v>
-      </c>
-      <c r="J26">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G27" s="7" t="s">
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" t="s">
+        <v>118</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="16">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" t="s">
+        <v>118</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="I27">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E28" t="s">
-        <v>73</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="I28">
-        <v>4</v>
-      </c>
-      <c r="J28">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" t="s">
-        <v>75</v>
-      </c>
-      <c r="D29" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" t="s">
-        <v>120</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="I30">
-        <v>100</v>
-      </c>
-      <c r="J30">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="16">
-      <c r="A31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" t="s">
-        <v>40</v>
-      </c>
-      <c r="E31" t="s">
-        <v>120</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="J31">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="5" t="s">
+      <c r="F34" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5" t="s">
+      <c r="D35" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>114</v>
+      <c r="E35" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Silkscreen + BOM fixes, added paste layers to gerbers
</commit_message>
<xml_diff>
--- a/Sprite/EagleCAD/Sprite/Sprite_Files/SpriteBOM.xlsx
+++ b/Sprite/EagleCAD/Sprite/Sprite_Files/SpriteBOM.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="SpriteBOM" localSheetId="0">Sheet1!$A$1:$G$31</definedName>
+    <definedName name="SpriteBOM" localSheetId="0">Sheet1!$A$1:$G$19</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="110">
   <si>
     <t>Part</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>10 nF</t>
   </si>
   <si>
@@ -72,42 +69,15 @@
     <t>Capacitor</t>
   </si>
   <si>
-    <t>C3</t>
-  </si>
-  <si>
     <t>470nF</t>
   </si>
   <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
     <t>2.2nF</t>
   </si>
   <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
     <t>100nF</t>
   </si>
   <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
     <t>C11</t>
   </si>
   <si>
@@ -120,18 +90,12 @@
     <t>4.7uF</t>
   </si>
   <si>
-    <t>JP2</t>
-  </si>
-  <si>
     <t>M02PTH</t>
   </si>
   <si>
     <t>1X02</t>
   </si>
   <si>
-    <t>JP3</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -153,15 +117,9 @@
     <t>LEDs</t>
   </si>
   <si>
-    <t>P1</t>
-  </si>
-  <si>
     <t>SPRITE_PIN</t>
   </si>
   <si>
-    <t>P2</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -183,24 +141,15 @@
     <t>47K</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
     <t>4.7K</t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
     <t>270R</t>
   </si>
   <si>
-    <t>R6</t>
-  </si>
-  <si>
     <t>R-US_R0805</t>
   </si>
   <si>
@@ -210,15 +159,9 @@
     <t>RESISTOR, American symbol</t>
   </si>
   <si>
-    <t>S1</t>
-  </si>
-  <si>
     <t>TASC</t>
   </si>
   <si>
-    <t>S2</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -267,12 +210,6 @@
     <t>TXC_7Z</t>
   </si>
   <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
     <t>0R</t>
   </si>
   <si>
@@ -393,9 +330,6 @@
     <t>1508-0-00-15-00-00-03-0</t>
   </si>
   <si>
-    <t>1508-0-00-15-00-00-03-1</t>
-  </si>
-  <si>
     <t>Test Pin</t>
   </si>
   <si>
@@ -408,23 +342,41 @@
     <t>0603-IND</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>R10</t>
+    <t>C1, C5, C9</t>
+  </si>
+  <si>
+    <t>C2, C3</t>
+  </si>
+  <si>
+    <t>C4, C7</t>
+  </si>
+  <si>
+    <t>C6, C8, C10</t>
+  </si>
+  <si>
+    <t>R3, R4</t>
+  </si>
+  <si>
+    <t>R6, R7, R8, R9, R10</t>
+  </si>
+  <si>
+    <t>S1, S2, S3, S4</t>
+  </si>
+  <si>
+    <t>P1, P2</t>
+  </si>
+  <si>
+    <t>JP2, JP3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -454,12 +406,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF555555"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -505,12 +451,12 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -523,7 +469,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -863,15 +808,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
@@ -897,332 +842,332 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
       <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>82</v>
+      <c r="F4" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>84</v>
+      <c r="F5" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>80</v>
+      <c r="F6" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
       <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>80</v>
+        <v>30</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B15" t="s">
-        <v>120</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1241,11 +1186,11 @@
       <c r="E16" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>97</v>
+      <c r="F16" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1256,426 +1201,106 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>99</v>
+        <v>48</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>101</v>
+        <v>52</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>101</v>
+        <v>55</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>124</v>
-      </c>
-      <c r="B24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" t="s">
-        <v>113</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" t="s">
-        <v>113</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" t="s">
-        <v>63</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="7" t="s">
+      <c r="A21" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="G29" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" t="s">
-        <v>74</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" t="s">
-        <v>118</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="16">
-      <c r="A33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" t="s">
-        <v>38</v>
-      </c>
-      <c r="E33" t="s">
-        <v>118</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>112</v>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>